<commit_message>
did some work, need to go to diff computer
</commit_message>
<xml_diff>
--- a/Final_Project_Workbook_Baseplate_Frame.xlsx
+++ b/Final_Project_Workbook_Baseplate_Frame.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smm9509\git\MCET150final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smm9509\vscode-cpp-projects\git\MCET150final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="10870" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="10875" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="List of Gages and Simulators" sheetId="16" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="107">
   <si>
     <t>#</t>
   </si>
@@ -393,22 +393,49 @@
     <t>Oil Embedded Flange Hole Position relative to A</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>the vertical height of this hole affects the angles at which the cylinder opens and closes its air hole.</t>
   </si>
   <si>
     <t>no, it is the void at the center of a hole.</t>
   </si>
   <si>
-    <t>a rectangle  0.1 in x 0.002 in, where the center of the entry point of the hole must be inside the rectangle</t>
-  </si>
-  <si>
     <t>Oil Embedded Flange Hole Position relative to D</t>
   </si>
   <si>
-    <t>N/A</t>
+    <t>Oil Embedded Flange Hole Size</t>
+  </si>
+  <si>
+    <t>go/nogo</t>
+  </si>
+  <si>
+    <t>the horizontal position of this hole affects the depth to which the piston moves during a stroke, and there is a lot of wiggle room available in the assembly for the depth to vary, so it has a large tolerance</t>
+  </si>
+  <si>
+    <t>a rectangular prism  0.1 in (horizontal) x 0.002 in (vertical) x 0.5 in (thick), where the axis of the hole must be inside the volume.</t>
+  </si>
+  <si>
+    <t>Height Gage, or a functional gage with a pin in the hole and the extension of the pin must fit in a slot</t>
+  </si>
+  <si>
+    <t>Cylinder Air Exhaust Hole Position</t>
+  </si>
+  <si>
+    <t>Cylinder Air Exhaust Hole Size</t>
+  </si>
+  <si>
+    <t>Height gage</t>
+  </si>
+  <si>
+    <t>The position of this hole affects when the exhaust occurs and how long it lasts.</t>
+  </si>
+  <si>
+    <t>C ,A</t>
+  </si>
+  <si>
+    <t>C, D</t>
+  </si>
+  <si>
+    <t>C, D, A</t>
   </si>
 </sst>
 </file>
@@ -645,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -735,20 +762,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -756,16 +813,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -774,31 +834,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,16 +1012,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>482147</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>43997</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>133226</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>584551</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>82698</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>552286</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -994,8 +1036,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="482147" y="133226"/>
-          <a:ext cx="7062004" cy="5105672"/>
+          <a:off x="653597" y="0"/>
+          <a:ext cx="10290628" cy="8019886"/>
           <a:chOff x="529772" y="130628"/>
           <a:chExt cx="6827054" cy="5283472"/>
         </a:xfrm>
@@ -1643,16 +1685,16 @@
   <dimension ref="B2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="18.6328125" customWidth="1"/>
+    <col min="2" max="4" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21" t="s">
         <v>54</v>
       </c>
@@ -1663,7 +1705,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>57</v>
       </c>
@@ -1674,7 +1716,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>60</v>
       </c>
@@ -1685,7 +1727,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>63</v>
       </c>
@@ -1696,7 +1738,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="23" t="s">
         <v>66</v>
       </c>
@@ -1707,7 +1749,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
         <v>68</v>
@@ -1716,7 +1758,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
         <v>69</v>
@@ -1725,7 +1767,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
         <v>70</v>
@@ -1734,35 +1776,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
       <c r="D15" s="24" t="s">
@@ -1779,154 +1821,154 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A31:X57"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="B34:I35"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.6328125" style="9" customWidth="1"/>
-    <col min="3" max="6" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="9" customWidth="1"/>
+    <col min="3" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.81640625" customWidth="1"/>
-    <col min="13" max="13" width="14.81640625" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="43.54296875" customWidth="1"/>
-    <col min="16" max="16" width="45.54296875" customWidth="1"/>
-    <col min="17" max="17" width="53.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.453125" customWidth="1"/>
-    <col min="20" max="20" width="12.81640625" customWidth="1"/>
+    <col min="15" max="15" width="43.5703125" customWidth="1"/>
+    <col min="16" max="16" width="45.5703125" customWidth="1"/>
+    <col min="17" max="17" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
     <col min="21" max="22" width="13" customWidth="1"/>
-    <col min="23" max="23" width="20.54296875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" style="2" customWidth="1"/>
     <col min="24" max="24" width="24" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.81640625" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" customWidth="1"/>
     <col min="26" max="26" width="15" customWidth="1"/>
-    <col min="27" max="27" width="10.54296875" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="34" t="s">
+    <row r="32" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="38" t="s">
+      <c r="D32" s="41"/>
+      <c r="E32" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="39"/>
-      <c r="G32" s="36" t="s">
+      <c r="F32" s="43"/>
+      <c r="G32" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H32" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="31"/>
+      <c r="I32" s="37"/>
       <c r="L32" s="2"/>
       <c r="M32" s="1"/>
       <c r="W32"/>
       <c r="X32"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A33" s="35"/>
-      <c r="B33" s="35"/>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
       <c r="L33" s="2"/>
       <c r="M33" s="1"/>
       <c r="W33"/>
       <c r="X33"/>
     </row>
-    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>1</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="30"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="30"/>
+      <c r="H34" s="50"/>
+      <c r="I34" s="50"/>
       <c r="L34" s="2"/>
       <c r="M34" s="1"/>
       <c r="W34"/>
       <c r="X34"/>
     </row>
-    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>2</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
+      <c r="H35" s="50"/>
+      <c r="I35" s="50"/>
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
       <c r="W35"/>
       <c r="X35"/>
     </row>
-    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>3</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
+      <c r="H36" s="50"/>
+      <c r="I36" s="50"/>
       <c r="L36" s="2"/>
       <c r="M36" s="1"/>
       <c r="W36"/>
       <c r="X36"/>
     </row>
-    <row r="37" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>4</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="28"/>
-      <c r="F37" s="29"/>
+      <c r="E37" s="48"/>
+      <c r="F37" s="49"/>
       <c r="G37" s="19"/>
-      <c r="H37" s="28"/>
-      <c r="I37" s="29"/>
+      <c r="H37" s="48"/>
+      <c r="I37" s="49"/>
       <c r="L37" s="2"/>
       <c r="M37" s="1"/>
       <c r="W37"/>
       <c r="X37"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>16</v>
       </c>
@@ -1936,7 +1978,7 @@
       <c r="W39"/>
       <c r="X39"/>
     </row>
-    <row r="40" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
@@ -1961,10 +2003,10 @@
       <c r="H40" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="32" t="s">
+      <c r="I40" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="J40" s="33"/>
+      <c r="J40" s="41"/>
       <c r="K40" s="12" t="s">
         <v>38</v>
       </c>
@@ -1976,7 +2018,7 @@
       <c r="W40"/>
       <c r="X40"/>
     </row>
-    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>1</v>
       </c>
@@ -1987,8 +2029,8 @@
       <c r="F41" s="8"/>
       <c r="G41" s="3"/>
       <c r="H41" s="5"/>
-      <c r="I41" s="28"/>
-      <c r="J41" s="29"/>
+      <c r="I41" s="48"/>
+      <c r="J41" s="49"/>
       <c r="K41" s="5"/>
       <c r="L41" s="11"/>
       <c r="R41" s="2"/>
@@ -1996,7 +2038,7 @@
       <c r="W41"/>
       <c r="X41"/>
     </row>
-    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>2</v>
       </c>
@@ -2007,8 +2049,8 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="5"/>
-      <c r="I42" s="28"/>
-      <c r="J42" s="29"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="49"/>
       <c r="K42" s="5"/>
       <c r="L42" s="11"/>
       <c r="R42" s="2"/>
@@ -2016,7 +2058,7 @@
       <c r="W42"/>
       <c r="X42"/>
     </row>
-    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>3</v>
       </c>
@@ -2027,8 +2069,8 @@
       <c r="F43" s="8"/>
       <c r="G43" s="14"/>
       <c r="H43" s="5"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="29"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="49"/>
       <c r="K43" s="5"/>
       <c r="L43" s="11"/>
       <c r="R43" s="2"/>
@@ -2036,7 +2078,7 @@
       <c r="W43"/>
       <c r="X43"/>
     </row>
-    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>4</v>
       </c>
@@ -2047,8 +2089,8 @@
       <c r="F44" s="8"/>
       <c r="G44" s="14"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="28"/>
-      <c r="J44" s="29"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="49"/>
       <c r="K44" s="5"/>
       <c r="L44" s="11"/>
       <c r="R44" s="2"/>
@@ -2056,7 +2098,7 @@
       <c r="W44"/>
       <c r="X44"/>
     </row>
-    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>5</v>
       </c>
@@ -2067,8 +2109,8 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="28"/>
-      <c r="J45" s="29"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="49"/>
       <c r="K45" s="5"/>
       <c r="L45" s="11"/>
       <c r="P45" s="2"/>
@@ -2076,7 +2118,7 @@
       <c r="W45"/>
       <c r="X45"/>
     </row>
-    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>6</v>
       </c>
@@ -2087,8 +2129,8 @@
       <c r="F46" s="3"/>
       <c r="G46" s="18"/>
       <c r="H46" s="5"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="29"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="49"/>
       <c r="K46" s="5"/>
       <c r="L46" s="11"/>
       <c r="P46" s="2"/>
@@ -2096,7 +2138,7 @@
       <c r="W46"/>
       <c r="X46"/>
     </row>
-    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>7</v>
       </c>
@@ -2107,8 +2149,8 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="5"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="29"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="49"/>
       <c r="K47" s="5"/>
       <c r="L47" s="11"/>
       <c r="P47" s="2"/>
@@ -2116,7 +2158,7 @@
       <c r="W47"/>
       <c r="X47"/>
     </row>
-    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>8</v>
       </c>
@@ -2127,8 +2169,8 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="5"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="29"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="49"/>
       <c r="K48" s="5"/>
       <c r="L48" s="11"/>
       <c r="P48" s="2"/>
@@ -2136,7 +2178,7 @@
       <c r="W48"/>
       <c r="X48"/>
     </row>
-    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>9</v>
       </c>
@@ -2147,8 +2189,8 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="29"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="49"/>
       <c r="K49" s="5"/>
       <c r="L49" s="11"/>
       <c r="P49" s="2"/>
@@ -2156,7 +2198,7 @@
       <c r="W49"/>
       <c r="X49"/>
     </row>
-    <row r="50" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>10</v>
       </c>
@@ -2167,8 +2209,8 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="5"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="29"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="49"/>
       <c r="K50" s="5"/>
       <c r="L50" s="11"/>
       <c r="P50" s="2"/>
@@ -2176,38 +2218,37 @@
       <c r="W50"/>
       <c r="X50"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M51" s="2"/>
       <c r="N51" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M53" s="2"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M54" s="2"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M55" s="2"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M56" s="2"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M57" s="2"/>
       <c r="N57" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="H32:I33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
     <mergeCell ref="I45:J45"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="H34:I34"/>
@@ -2222,11 +2263,12 @@
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="H35:I35"/>
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2239,87 +2281,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A31:Z58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.6328125" style="9" customWidth="1"/>
-    <col min="3" max="6" width="10.6328125" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="9" customWidth="1"/>
+    <col min="3" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="35.28515625" customWidth="1"/>
     <col min="8" max="9" width="14" customWidth="1"/>
-    <col min="11" max="11" width="25.453125" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" customWidth="1"/>
-    <col min="13" max="13" width="20.81640625" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="52.81640625" customWidth="1"/>
-    <col min="15" max="15" width="14.81640625" customWidth="1"/>
+    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="52.85546875" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="43.54296875" customWidth="1"/>
-    <col min="18" max="18" width="45.54296875" customWidth="1"/>
-    <col min="19" max="19" width="53.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12.453125" customWidth="1"/>
-    <col min="22" max="22" width="12.81640625" customWidth="1"/>
+    <col min="17" max="17" width="43.5703125" customWidth="1"/>
+    <col min="18" max="18" width="45.5703125" customWidth="1"/>
+    <col min="19" max="19" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="12.42578125" customWidth="1"/>
+    <col min="22" max="22" width="12.85546875" customWidth="1"/>
     <col min="23" max="24" width="13" customWidth="1"/>
-    <col min="25" max="25" width="20.54296875" style="2" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" style="2" customWidth="1"/>
     <col min="26" max="26" width="24" style="1" customWidth="1"/>
-    <col min="27" max="27" width="15.81640625" customWidth="1"/>
+    <col min="27" max="27" width="15.85546875" customWidth="1"/>
     <col min="28" max="28" width="15" customWidth="1"/>
-    <col min="29" max="29" width="10.54296875" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="34" t="s">
+    <row r="32" spans="1:26" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="38" t="s">
+      <c r="D32" s="41"/>
+      <c r="E32" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="39"/>
-      <c r="G32" s="36" t="s">
+      <c r="F32" s="43"/>
+      <c r="G32" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="38" t="s">
+      <c r="H32" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="39"/>
+      <c r="I32" s="43"/>
       <c r="N32" s="2"/>
       <c r="O32" s="1"/>
       <c r="Y32"/>
       <c r="Z32"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A33" s="35"/>
-      <c r="B33" s="35"/>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="41"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="44"/>
+      <c r="I33" s="45"/>
       <c r="N33" s="2"/>
       <c r="O33" s="1"/>
       <c r="Y33"/>
       <c r="Z33"/>
     </row>
-    <row r="34" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>1</v>
       </c>
@@ -2332,23 +2374,23 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="F34" s="30"/>
+      <c r="F34" s="50"/>
       <c r="G34" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="42" t="s">
+      <c r="H34" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="I34" s="43"/>
+      <c r="I34" s="54"/>
       <c r="N34" s="2"/>
       <c r="O34" s="1"/>
       <c r="Y34"/>
       <c r="Z34"/>
     </row>
-    <row r="35" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>2</v>
       </c>
@@ -2361,23 +2403,23 @@
       <c r="D35" s="5">
         <v>2</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="F35" s="30"/>
+      <c r="F35" s="50"/>
       <c r="G35" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H35" s="42" t="s">
+      <c r="H35" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="I35" s="43"/>
+      <c r="I35" s="54"/>
       <c r="N35" s="2"/>
       <c r="O35" s="1"/>
       <c r="Y35"/>
       <c r="Z35"/>
     </row>
-    <row r="36" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>3</v>
       </c>
@@ -2390,23 +2432,23 @@
       <c r="D36" s="5">
         <v>2</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E36" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="F36" s="30"/>
+      <c r="F36" s="50"/>
       <c r="G36" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H36" s="42" t="s">
+      <c r="H36" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="I36" s="43"/>
+      <c r="I36" s="54"/>
       <c r="N36" s="2"/>
       <c r="O36" s="1"/>
       <c r="Y36"/>
       <c r="Z36"/>
     </row>
-    <row r="37" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>4</v>
       </c>
@@ -2419,37 +2461,37 @@
       <c r="D37" s="5">
         <v>2</v>
       </c>
-      <c r="E37" s="28" t="s">
+      <c r="E37" s="48" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="29"/>
+      <c r="F37" s="49"/>
       <c r="G37" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="H37" s="42" t="s">
+      <c r="H37" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="I37" s="43"/>
+      <c r="I37" s="54"/>
       <c r="N37" s="2"/>
       <c r="O37" s="1"/>
       <c r="Y37"/>
       <c r="Z37"/>
     </row>
-    <row r="39" spans="1:26" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:26" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="12"/>
-      <c r="I39" s="32" t="s">
+      <c r="I39" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="33"/>
+      <c r="J39" s="41"/>
       <c r="V39" s="2"/>
       <c r="W39" s="1"/>
       <c r="Y39"/>
       <c r="Z39"/>
     </row>
-    <row r="40" spans="1:26" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:26" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
@@ -2480,10 +2522,10 @@
       <c r="J40" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="32" t="s">
+      <c r="K40" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="L40" s="33"/>
+      <c r="L40" s="41"/>
       <c r="M40" s="27" t="s">
         <v>38</v>
       </c>
@@ -2495,318 +2537,511 @@
       <c r="Y40"/>
       <c r="Z40"/>
     </row>
-    <row r="41" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>1</v>
       </c>
       <c r="B41" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D41" s="48"/>
-      <c r="E41" s="48"/>
-      <c r="F41" s="48"/>
-      <c r="G41" s="44" t="s">
-        <v>51</v>
-      </c>
-      <c r="H41" s="44" t="s">
+      <c r="C41" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="56">
+        <v>2E-3</v>
+      </c>
+      <c r="E41" s="56">
+        <f>E43-D41</f>
+        <v>0.37424999999999997</v>
+      </c>
+      <c r="F41" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" s="31" t="s">
+        <v>104</v>
+      </c>
+      <c r="I41" s="3">
+        <v>2</v>
+      </c>
+      <c r="J41" s="5">
+        <v>2</v>
+      </c>
+      <c r="K41" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="I41" s="3">
-        <f>C35</f>
-        <v>1</v>
-      </c>
-      <c r="J41" s="5">
-        <f>D35</f>
-        <v>2</v>
-      </c>
-      <c r="K41" s="28" t="s">
+      <c r="L41" s="49"/>
+      <c r="M41" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="L41" s="29"/>
-      <c r="M41" s="50" t="s">
-        <v>94</v>
-      </c>
       <c r="N41" s="51" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="T41" s="2"/>
       <c r="U41" s="1"/>
       <c r="Y41"/>
       <c r="Z41"/>
     </row>
-    <row r="42" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
+        <f>A41+1</f>
         <v>2</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="E42" s="56">
+        <f>E43-D42</f>
+        <v>0.27625</v>
+      </c>
+      <c r="F42" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="57" t="str">
+        <f>G41</f>
+        <v>Height Gage, or a functional gage with a pin in the hole and the extension of the pin must fit in a slot</v>
+      </c>
+      <c r="H42" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="I42" s="3">
+        <v>2</v>
+      </c>
+      <c r="J42" s="5">
+        <v>2</v>
+      </c>
+      <c r="K42" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="D42" s="48"/>
-      <c r="E42" s="48"/>
-      <c r="F42" s="48"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="44"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="5"/>
-      <c r="K42" s="28"/>
-      <c r="L42" s="29"/>
-      <c r="M42" s="50"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="36" t="str">
+        <f>M41</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
       <c r="N42" s="52"/>
       <c r="T42" s="2"/>
       <c r="U42" s="1"/>
       <c r="Y42"/>
       <c r="Z42"/>
     </row>
-    <row r="43" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
+        <f t="shared" ref="A43:A56" si="0">A42+1</f>
         <v>3</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="48">
+      <c r="B43" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="55">
+        <v>0.377</v>
+      </c>
+      <c r="D43" s="56">
         <f>-F43+E43</f>
         <v>1.3499999999999623E-3</v>
       </c>
-      <c r="E43" s="47">
+      <c r="E43" s="55">
         <v>0.37624999999999997</v>
       </c>
-      <c r="F43" s="47">
+      <c r="F43" s="34">
         <v>0.37490000000000001</v>
       </c>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
+      <c r="G43" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="H43" s="32" t="s">
+        <v>7</v>
+      </c>
       <c r="I43" s="14"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="28"/>
-      <c r="L43" s="29"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="11"/>
+      <c r="K43" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="L43" s="49"/>
+      <c r="M43" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="N43" s="30" t="s">
+        <v>47</v>
+      </c>
       <c r="T43" s="2"/>
       <c r="U43" s="1"/>
       <c r="Y43"/>
       <c r="Z43"/>
     </row>
-    <row r="44" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B44" s="16"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="48"/>
-      <c r="E44" s="47"/>
-      <c r="F44" s="47"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
+      <c r="B44" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="55">
+        <v>0.159</v>
+      </c>
+      <c r="D44" s="56">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E44" s="55">
+        <f>C44-D44</f>
+        <v>0.154</v>
+      </c>
+      <c r="F44" s="55">
+        <f>C44+D44</f>
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="G44" s="57" t="str">
+        <f>G43</f>
+        <v>go/nogo</v>
+      </c>
+      <c r="H44" s="32" t="str">
+        <f>H43</f>
+        <v>NA</v>
+      </c>
       <c r="I44" s="14"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="29"/>
-      <c r="M44" s="50"/>
-      <c r="N44" s="11"/>
+      <c r="K44" s="48" t="str">
+        <f>K43</f>
+        <v>NA</v>
+      </c>
+      <c r="L44" s="49"/>
+      <c r="M44" s="36" t="str">
+        <f>M43</f>
+        <v>yes</v>
+      </c>
+      <c r="N44" s="11" t="str">
+        <f>N43</f>
+        <v>The Size of the feature cannot be any bigger than MMC and no smaller than Min.</v>
+      </c>
       <c r="T44" s="2"/>
       <c r="U44" s="1"/>
       <c r="Y44"/>
       <c r="Z44"/>
     </row>
-    <row r="45" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B45" s="16"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="48"/>
-      <c r="E45" s="48"/>
-      <c r="F45" s="48"/>
-      <c r="G45" s="44"/>
-      <c r="H45" s="44"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="5"/>
-      <c r="K45" s="28"/>
-      <c r="L45" s="29"/>
-      <c r="M45" s="50"/>
-      <c r="N45" s="11"/>
+      <c r="B45" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="55" t="str">
+        <f>C42</f>
+        <v>NA</v>
+      </c>
+      <c r="D45" s="56">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E45" s="56">
+        <f>E44-D45</f>
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="F45" s="56" t="str">
+        <f>F42</f>
+        <v>NA</v>
+      </c>
+      <c r="G45" s="57" t="s">
+        <v>102</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="I45" s="3">
+        <v>3</v>
+      </c>
+      <c r="J45" s="5">
+        <v>3</v>
+      </c>
+      <c r="K45" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="L45" s="49"/>
+      <c r="M45" s="36" t="str">
+        <f>M42</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
+      <c r="N45" s="30" t="str">
+        <f>"The axis of the feature must fall within a cylindrical tolerance zone with a diameter of "&amp;D45&amp;".  The zone will be located relative to the Datums by the basic dimensions."</f>
+        <v>The axis of the feature must fall within a cylindrical tolerance zone with a diameter of 0.005.  The zone will be located relative to the Datums by the basic dimensions.</v>
+      </c>
       <c r="R45" s="2"/>
       <c r="S45" s="1"/>
       <c r="Y45"/>
       <c r="Z45"/>
     </row>
-    <row r="46" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B46" s="16"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="48"/>
-      <c r="E46" s="48"/>
-      <c r="F46" s="48"/>
-      <c r="G46" s="46"/>
-      <c r="H46" s="46"/>
+      <c r="C46" s="55"/>
+      <c r="D46" s="56"/>
+      <c r="E46" s="56"/>
+      <c r="F46" s="56"/>
+      <c r="G46" s="57"/>
+      <c r="H46" s="33"/>
       <c r="I46" s="18"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="50"/>
+      <c r="K46" s="48"/>
+      <c r="L46" s="49"/>
+      <c r="M46" s="36"/>
       <c r="N46" s="11"/>
       <c r="R46" s="2"/>
       <c r="S46" s="1"/>
       <c r="Y46"/>
       <c r="Z46"/>
     </row>
-    <row r="47" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B47" s="16"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="48"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="48"/>
-      <c r="G47" s="44"/>
-      <c r="H47" s="44"/>
-      <c r="I47" s="3"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="56"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="56"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="18"/>
       <c r="J47" s="5"/>
       <c r="K47" s="28"/>
       <c r="L47" s="29"/>
-      <c r="M47" s="50"/>
-      <c r="N47" s="11"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="30"/>
       <c r="R47" s="2"/>
       <c r="S47" s="1"/>
       <c r="Y47"/>
       <c r="Z47"/>
     </row>
-    <row r="48" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B48" s="16"/>
-      <c r="C48" s="17"/>
-      <c r="D48" s="48"/>
-      <c r="E48" s="48"/>
-      <c r="F48" s="48"/>
-      <c r="G48" s="44"/>
-      <c r="H48" s="44"/>
-      <c r="I48" s="3"/>
+      <c r="C48" s="55"/>
+      <c r="D48" s="56"/>
+      <c r="E48" s="56"/>
+      <c r="F48" s="56"/>
+      <c r="G48" s="57"/>
+      <c r="H48" s="33"/>
+      <c r="I48" s="18"/>
       <c r="J48" s="5"/>
       <c r="K48" s="28"/>
       <c r="L48" s="29"/>
-      <c r="M48" s="50"/>
-      <c r="N48" s="11"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="30"/>
       <c r="R48" s="2"/>
       <c r="S48" s="1"/>
       <c r="Y48"/>
       <c r="Z48"/>
     </row>
-    <row r="49" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B49" s="16"/>
-      <c r="C49" s="17"/>
-      <c r="D49" s="48"/>
-      <c r="E49" s="48"/>
-      <c r="F49" s="48"/>
-      <c r="G49" s="44"/>
-      <c r="H49" s="44"/>
-      <c r="I49" s="3"/>
+      <c r="C49" s="55"/>
+      <c r="D49" s="56"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="57"/>
+      <c r="H49" s="33"/>
+      <c r="I49" s="18"/>
       <c r="J49" s="5"/>
       <c r="K49" s="28"/>
       <c r="L49" s="29"/>
-      <c r="M49" s="50"/>
-      <c r="N49" s="11"/>
+      <c r="M49" s="36"/>
+      <c r="N49" s="30"/>
       <c r="R49" s="2"/>
       <c r="S49" s="1"/>
       <c r="Y49"/>
       <c r="Z49"/>
     </row>
-    <row r="50" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B50" s="16"/>
-      <c r="C50" s="17"/>
-      <c r="D50" s="48"/>
-      <c r="E50" s="48"/>
-      <c r="F50" s="48"/>
-      <c r="G50" s="44"/>
-      <c r="H50" s="44"/>
-      <c r="I50" s="3"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="56"/>
+      <c r="E50" s="56"/>
+      <c r="F50" s="56"/>
+      <c r="G50" s="57"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="18"/>
       <c r="J50" s="5"/>
       <c r="K50" s="28"/>
       <c r="L50" s="29"/>
-      <c r="M50" s="50"/>
-      <c r="N50" s="26"/>
+      <c r="M50" s="36"/>
+      <c r="N50" s="30"/>
       <c r="R50" s="2"/>
       <c r="S50" s="1"/>
       <c r="Y50"/>
       <c r="Z50"/>
     </row>
-    <row r="51" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B51" s="16"/>
-      <c r="C51" s="17"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="44"/>
-      <c r="H51" s="44"/>
-      <c r="I51" s="3"/>
+      <c r="C51" s="55"/>
+      <c r="D51" s="56"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="56"/>
+      <c r="G51" s="57"/>
+      <c r="H51" s="33"/>
+      <c r="I51" s="18"/>
       <c r="J51" s="5"/>
       <c r="K51" s="28"/>
       <c r="L51" s="29"/>
-      <c r="M51" s="50"/>
-      <c r="N51" s="11"/>
+      <c r="M51" s="36"/>
+      <c r="N51" s="30"/>
       <c r="R51" s="2"/>
       <c r="S51" s="1"/>
       <c r="Y51"/>
       <c r="Z51"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="O52" s="2"/>
-      <c r="P52" s="1"/>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="O54" s="2"/>
-      <c r="P54" s="1"/>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="O55" s="2"/>
-      <c r="P55" s="1"/>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="O56" s="2"/>
-      <c r="P56" s="1"/>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B52" s="16"/>
+      <c r="C52" s="55"/>
+      <c r="D52" s="56"/>
+      <c r="E52" s="56"/>
+      <c r="F52" s="56"/>
+      <c r="G52" s="57"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="18"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="29"/>
+      <c r="M52" s="36"/>
+      <c r="N52" s="30"/>
+      <c r="R52" s="2"/>
+      <c r="S52" s="1"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
+    </row>
+    <row r="53" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B53" s="16"/>
+      <c r="C53" s="55"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="57"/>
+      <c r="H53" s="33"/>
+      <c r="I53" s="18"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="29"/>
+      <c r="M53" s="36"/>
+      <c r="N53" s="30"/>
+      <c r="R53" s="2"/>
+      <c r="S53" s="1"/>
+      <c r="Y53"/>
+      <c r="Z53"/>
+    </row>
+    <row r="54" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B54" s="16"/>
+      <c r="C54" s="55"/>
+      <c r="D54" s="56"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="56"/>
+      <c r="G54" s="57"/>
+      <c r="H54" s="33"/>
+      <c r="I54" s="18"/>
+      <c r="J54" s="5"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="29"/>
+      <c r="M54" s="36"/>
+      <c r="N54" s="30"/>
+      <c r="R54" s="2"/>
+      <c r="S54" s="1"/>
+      <c r="Y54"/>
+      <c r="Z54"/>
+    </row>
+    <row r="55" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B55" s="16"/>
+      <c r="C55" s="55"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="56"/>
+      <c r="F55" s="56"/>
+      <c r="G55" s="57"/>
+      <c r="H55" s="33"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="5"/>
+      <c r="K55" s="28"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="36"/>
+      <c r="N55" s="30"/>
+      <c r="R55" s="2"/>
+      <c r="S55" s="1"/>
+      <c r="Y55"/>
+      <c r="Z55"/>
+    </row>
+    <row r="56" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B56" s="16"/>
+      <c r="C56" s="55"/>
+      <c r="D56" s="56"/>
+      <c r="E56" s="56"/>
+      <c r="F56" s="56"/>
+      <c r="G56" s="57"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="18"/>
+      <c r="J56" s="5"/>
+      <c r="K56" s="28"/>
+      <c r="L56" s="29"/>
+      <c r="M56" s="36"/>
+      <c r="N56" s="30"/>
+      <c r="R56" s="2"/>
+      <c r="S56" s="1"/>
+      <c r="Y56"/>
+      <c r="Z56"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O57" s="2"/>
       <c r="P57" s="1"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="O58" s="2"/>
       <c r="P58" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="H32:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:G33"/>
+  <mergeCells count="23">
+    <mergeCell ref="K46:L46"/>
     <mergeCell ref="K45:L45"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
@@ -2816,12 +3051,19 @@
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="K44:L44"/>
-    <mergeCell ref="K46:L46"/>
-    <mergeCell ref="K47:L47"/>
-    <mergeCell ref="K48:L48"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K51:L51"/>
-    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2834,86 +3076,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A31:X56"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView topLeftCell="G37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="25.6328125" style="9" customWidth="1"/>
-    <col min="3" max="6" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="9" customWidth="1"/>
+    <col min="3" max="6" width="10.5703125" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.453125" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" customWidth="1"/>
-    <col min="11" max="11" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.81640625" customWidth="1"/>
-    <col min="13" max="13" width="14.81640625" customWidth="1"/>
+    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="43.54296875" customWidth="1"/>
-    <col min="16" max="16" width="45.54296875" customWidth="1"/>
-    <col min="17" max="17" width="53.81640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.453125" customWidth="1"/>
-    <col min="20" max="20" width="12.81640625" customWidth="1"/>
+    <col min="15" max="15" width="43.5703125" customWidth="1"/>
+    <col min="16" max="16" width="45.5703125" customWidth="1"/>
+    <col min="17" max="17" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
     <col min="21" max="22" width="13" customWidth="1"/>
-    <col min="23" max="23" width="20.54296875" style="2" customWidth="1"/>
+    <col min="23" max="23" width="20.5703125" style="2" customWidth="1"/>
     <col min="24" max="24" width="24" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.81640625" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" customWidth="1"/>
     <col min="26" max="26" width="15" customWidth="1"/>
-    <col min="27" max="27" width="10.54296875" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="34" t="s">
+    <row r="32" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="33"/>
-      <c r="E32" s="38" t="s">
+      <c r="D32" s="41"/>
+      <c r="E32" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="39"/>
-      <c r="G32" s="36" t="s">
+      <c r="F32" s="43"/>
+      <c r="G32" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="31" t="s">
+      <c r="H32" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="31"/>
+      <c r="I32" s="37"/>
       <c r="L32" s="2"/>
       <c r="M32" s="1"/>
       <c r="W32"/>
       <c r="X32"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A33" s="35"/>
-      <c r="B33" s="35"/>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A33" s="39"/>
+      <c r="B33" s="39"/>
       <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
+      <c r="E33" s="44"/>
+      <c r="F33" s="45"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
       <c r="L33" s="2"/>
       <c r="M33" s="1"/>
       <c r="W33"/>
       <c r="X33"/>
     </row>
-    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>1</v>
       </c>
@@ -2926,23 +3168,23 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="30"/>
+      <c r="F34" s="50"/>
       <c r="G34" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="H34" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="30"/>
+      <c r="I34" s="50"/>
       <c r="L34" s="2"/>
       <c r="M34" s="1"/>
       <c r="W34"/>
       <c r="X34"/>
     </row>
-    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>2</v>
       </c>
@@ -2955,23 +3197,23 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="30"/>
+      <c r="F35" s="50"/>
       <c r="G35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="30" t="s">
+      <c r="H35" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="30"/>
+      <c r="I35" s="50"/>
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
       <c r="W35"/>
       <c r="X35"/>
     </row>
-    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>3</v>
       </c>
@@ -2984,23 +3226,23 @@
       <c r="D36" s="5">
         <v>0</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E36" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="30"/>
+      <c r="F36" s="50"/>
       <c r="G36" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="30" t="s">
+      <c r="H36" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="I36" s="30"/>
+      <c r="I36" s="50"/>
       <c r="L36" s="2"/>
       <c r="M36" s="1"/>
       <c r="W36"/>
       <c r="X36"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
@@ -3010,7 +3252,7 @@
       <c r="W38"/>
       <c r="X38"/>
     </row>
-    <row r="39" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -3035,10 +3277,10 @@
       <c r="H39" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="32" t="s">
+      <c r="I39" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="J39" s="33"/>
+      <c r="J39" s="41"/>
       <c r="K39" s="27" t="s">
         <v>38</v>
       </c>
@@ -3050,7 +3292,7 @@
       <c r="W39"/>
       <c r="X39"/>
     </row>
-    <row r="40" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>1</v>
       </c>
@@ -3075,10 +3317,10 @@
       <c r="H40" s="5">
         <v>0</v>
       </c>
-      <c r="I40" s="28" t="s">
+      <c r="I40" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="J40" s="29"/>
+      <c r="J40" s="49"/>
       <c r="K40" s="5" t="s">
         <v>77</v>
       </c>
@@ -3090,7 +3332,7 @@
       <c r="W40"/>
       <c r="X40"/>
     </row>
-    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>2</v>
       </c>
@@ -3117,10 +3359,10 @@
       <c r="H41" s="5">
         <v>0</v>
       </c>
-      <c r="I41" s="28" t="s">
+      <c r="I41" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J41" s="29"/>
+      <c r="J41" s="49"/>
       <c r="K41" s="5" t="s">
         <v>15</v>
       </c>
@@ -3132,7 +3374,7 @@
       <c r="W41"/>
       <c r="X41"/>
     </row>
-    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>3</v>
       </c>
@@ -3157,10 +3399,10 @@
       <c r="H42" s="5">
         <v>1</v>
       </c>
-      <c r="I42" s="28" t="s">
+      <c r="I42" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="29"/>
+      <c r="J42" s="49"/>
       <c r="K42" s="5" t="s">
         <v>15</v>
       </c>
@@ -3172,7 +3414,7 @@
       <c r="W42"/>
       <c r="X42"/>
     </row>
-    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>4</v>
       </c>
@@ -3197,10 +3439,10 @@
       <c r="H43" s="5">
         <v>2</v>
       </c>
-      <c r="I43" s="28" t="s">
+      <c r="I43" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="J43" s="29"/>
+      <c r="J43" s="49"/>
       <c r="K43" s="5" t="s">
         <v>77</v>
       </c>
@@ -3212,7 +3454,7 @@
       <c r="W43"/>
       <c r="X43"/>
     </row>
-    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>5</v>
       </c>
@@ -3239,10 +3481,10 @@
       <c r="H44" s="5">
         <v>0</v>
       </c>
-      <c r="I44" s="28" t="s">
+      <c r="I44" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J44" s="29"/>
+      <c r="J44" s="49"/>
       <c r="K44" s="5" t="s">
         <v>15</v>
       </c>
@@ -3254,7 +3496,7 @@
       <c r="W44"/>
       <c r="X44"/>
     </row>
-    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>6</v>
       </c>
@@ -3280,10 +3522,10 @@
       <c r="H45" s="5">
         <v>2</v>
       </c>
-      <c r="I45" s="28" t="s">
+      <c r="I45" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="J45" s="29"/>
+      <c r="J45" s="49"/>
       <c r="K45" s="5" t="s">
         <v>15</v>
       </c>
@@ -3295,7 +3537,7 @@
       <c r="W45"/>
       <c r="X45"/>
     </row>
-    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>7</v>
       </c>
@@ -3320,10 +3562,10 @@
       <c r="H46" s="5">
         <v>3</v>
       </c>
-      <c r="I46" s="28" t="s">
+      <c r="I46" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="J46" s="29"/>
+      <c r="J46" s="49"/>
       <c r="K46" s="5" t="s">
         <v>76</v>
       </c>
@@ -3335,7 +3577,7 @@
       <c r="W46"/>
       <c r="X46"/>
     </row>
-    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>8</v>
       </c>
@@ -3346,8 +3588,8 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="5"/>
-      <c r="I47" s="28"/>
-      <c r="J47" s="29"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="49"/>
       <c r="K47" s="5"/>
       <c r="L47" s="26"/>
       <c r="P47" s="2"/>
@@ -3355,7 +3597,7 @@
       <c r="W47"/>
       <c r="X47"/>
     </row>
-    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>9</v>
       </c>
@@ -3366,8 +3608,8 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="5"/>
-      <c r="I48" s="28"/>
-      <c r="J48" s="29"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="49"/>
       <c r="K48" s="5"/>
       <c r="L48" s="26"/>
       <c r="P48" s="2"/>
@@ -3375,7 +3617,7 @@
       <c r="W48"/>
       <c r="X48"/>
     </row>
-    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>10</v>
       </c>
@@ -3386,8 +3628,8 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="28"/>
-      <c r="J49" s="29"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="49"/>
       <c r="K49" s="5"/>
       <c r="L49" s="26"/>
       <c r="P49" s="2"/>
@@ -3395,32 +3637,43 @@
       <c r="W49"/>
       <c r="X49"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M50" s="2"/>
       <c r="N50" s="1"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M52" s="2"/>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M53" s="2"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M54" s="2"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M55" s="2"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M56" s="2"/>
       <c r="N56" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="E34:F34"/>
     <mergeCell ref="I49:J49"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H35:I35"/>
@@ -3432,18 +3685,7 @@
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="I47:J47"/>
     <mergeCell ref="I48:J48"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="H32:I33"/>
     <mergeCell ref="I41:J41"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="E34:F34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
finished frame drawing and workbook
</commit_message>
<xml_diff>
--- a/Final_Project_Workbook_Baseplate_Frame.xlsx
+++ b/Final_Project_Workbook_Baseplate_Frame.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smm9509\vscode-cpp-projects\git\MCET150final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smm9509\git\MCET150final\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28785" windowHeight="10875" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28790" windowHeight="10880" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="List of Gages and Simulators" sheetId="16" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="154">
   <si>
     <t>#</t>
   </si>
@@ -366,9 +366,6 @@
     <t>A - bottom face</t>
   </si>
   <si>
-    <t>flat face of part</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -378,9 +375,6 @@
     <t xml:space="preserve">C - front face </t>
   </si>
   <si>
-    <t>threaded pin gage with a ground cylinder on its end</t>
-  </si>
-  <si>
     <t>enforce perpendicularity to face</t>
   </si>
   <si>
@@ -414,21 +408,12 @@
     <t>a rectangular prism  0.1 in (horizontal) x 0.002 in (vertical) x 0.5 in (thick), where the axis of the hole must be inside the volume.</t>
   </si>
   <si>
-    <t>Height Gage, or a functional gage with a pin in the hole and the extension of the pin must fit in a slot</t>
-  </si>
-  <si>
     <t>Cylinder Air Exhaust Hole Position</t>
   </si>
   <si>
     <t>Cylinder Air Exhaust Hole Size</t>
   </si>
   <si>
-    <t>Height gage</t>
-  </si>
-  <si>
-    <t>The position of this hole affects when the exhaust occurs and how long it lasts.</t>
-  </si>
-  <si>
     <t>C ,A</t>
   </si>
   <si>
@@ -436,6 +421,162 @@
   </si>
   <si>
     <t>C, D, A</t>
+  </si>
+  <si>
+    <t>Pressurized Air Intake Threaded Hole Size</t>
+  </si>
+  <si>
+    <t>NA (threaded)</t>
+  </si>
+  <si>
+    <t>Gage pin + Height gage</t>
+  </si>
+  <si>
+    <t>Gage pin + Height Gage, or a functional gage with a pin in the hole and the extension of the pin must fit in a slot</t>
+  </si>
+  <si>
+    <t>thread gage</t>
+  </si>
+  <si>
+    <t>The position of this threaded hole affects the position of the part that goes inside the hole, which has another hole inside it, and the position of that hole controls when the air intake occurs and how long it lasts.</t>
+  </si>
+  <si>
+    <t>the shape of thread gage must fit inside the threaded hole and not wiggle too much</t>
+  </si>
+  <si>
+    <t>Pressurized Air Intake Threaded Hole Position</t>
+  </si>
+  <si>
+    <t>thread gage + height gage</t>
+  </si>
+  <si>
+    <t>yes, it's the size of a hole</t>
+  </si>
+  <si>
+    <t>The position of this hole affects when the exhaust occurs and how long it lasts. The hole does not need to be perpendicular to datum C, it could even be parallel and the vent will still work.</t>
+  </si>
+  <si>
+    <t>thread gage + dial indicator</t>
+  </si>
+  <si>
+    <t>no, it is a single surface</t>
+  </si>
+  <si>
+    <t>gage pin + dial indicator</t>
+  </si>
+  <si>
+    <t>Cylinder Air Exhaust Hole Paralellism</t>
+  </si>
+  <si>
+    <t>the space between two parallel planes, perpendicular to datum C and parallel to datum A, 0.05 in apart, the 0.5 in long axis of this hole must be between them</t>
+  </si>
+  <si>
+    <t>Pressurized Air Intake Threaded Hole Parallellism</t>
+  </si>
+  <si>
+    <t>A, C</t>
+  </si>
+  <si>
+    <t>The vertical angle of this hole affects the vertical ovalness of the end of the hole, which needs to be controlled to affect the range along the vertical axis where exhausting can occur.</t>
+  </si>
+  <si>
+    <t>The position of this hole affects the alignment with the two airflow holes, which affects the timing of the intake and exhaust</t>
+  </si>
+  <si>
+    <t>Bottom face perpendicularity to C</t>
+  </si>
+  <si>
+    <t>dial indicator</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>I think that the maximum tilt side-to-side of the assembly relative to the base is about 5.7 degrees (tan(5.7) = .1)</t>
+  </si>
+  <si>
+    <t>no, it is a surface.</t>
+  </si>
+  <si>
+    <t>two planes both perpendicular to datum C</t>
+  </si>
+  <si>
+    <t>Bottom face perpendicularity to D</t>
+  </si>
+  <si>
+    <t>I think that the maximum tilt back-and-forth of the assembly relative to the base is about 1.72 degrees (tan(1.72) = .03)</t>
+  </si>
+  <si>
+    <t>two planes both perpendicular to datum D</t>
+  </si>
+  <si>
+    <t>Paralellness of surface oposite datum C</t>
+  </si>
+  <si>
+    <t>The two air holes rely on this surface and they need to be really precise, so this surface needs to be parallel. Also, it needs to be really flat so that the cylinder can slide against it.</t>
+  </si>
+  <si>
+    <t>two places parallel to datum C</t>
+  </si>
+  <si>
+    <t>angle block or surface plate on flat face of part</t>
+  </si>
+  <si>
+    <t>Threaded hole for baseplate bolt size</t>
+  </si>
+  <si>
+    <t>.5, 1, 1.9</t>
+  </si>
+  <si>
+    <t>.5, 1, 2.1</t>
+  </si>
+  <si>
+    <t>.5, 1, 2.0</t>
+  </si>
+  <si>
+    <t>hole for cylinder bolt size</t>
+  </si>
+  <si>
+    <t>hole for cylinder bolt position</t>
+  </si>
+  <si>
+    <t>RC9 because the bolt size varies so much</t>
+  </si>
+  <si>
+    <t>go-nogo, or just push the bolt into the hole to make sure it fits and doesn't wiggle</t>
+  </si>
+  <si>
+    <t>this is the maximum distance the hole can be translated without penetrating the two big faces of the part</t>
+  </si>
+  <si>
+    <t>this is the maximum distance the hole can be translated without penetrating the two side faces of the part</t>
+  </si>
+  <si>
+    <t>Threaded hole for baseplate bolt position to B</t>
+  </si>
+  <si>
+    <t>two thread gages + calipers</t>
+  </si>
+  <si>
+    <t>a rectangular prism  0.2 in (horizontal) x 0.05 in (vertical) x 0.5 in (projected) projected down from the surface of the hole, where the axis of the hole must be inside the prism.</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>the distance between the two holes needs to be really precise</t>
+  </si>
+  <si>
+    <t>two concentric cylinders around datum B, both cylinders projected out of the surface 0.5 in, the inner cylinder is 3.498 in diameter and the outer cylinder is 3.502 in diameter, and the axis needs to pass through the volume between the cylinders</t>
+  </si>
+  <si>
+    <t>Threaded hole for baseplate bolt perpendicularity to C, D</t>
+  </si>
+  <si>
+    <t>the distance between the two holes needs to stay precise along the whole projected length</t>
+  </si>
+  <si>
+    <t>a cylinder centered on the true position of the hole, perpendicular to datums C and D, projected 0.5 in from the surface, and the axis of the hole needs to go through the whole length of the cylinder.</t>
   </si>
 </sst>
 </file>
@@ -672,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -753,6 +894,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -762,22 +933,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -789,12 +948,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -813,15 +966,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -835,12 +979,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -936,75 +1074,44 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>554181</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>69272</xdr:rowOff>
+      <xdr:colOff>285290</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>73624</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="8154988" cy="4651374"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FAC05C7-631B-4FF2-9579-48F00B3EE306}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1829754</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>53964</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="554181" y="450272"/>
-          <a:ext cx="8154988" cy="4651374"/>
+          <a:off x="285290" y="73624"/>
+          <a:ext cx="6882145" cy="5318021"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
       </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="9600"/>
-            <a:t>Place Picture of drawing here</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="9600">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+    </xdr:pic>
     <xdr:clientData/>
-  </xdr:oneCellAnchor>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1037,7 +1144,7 @@
       <xdr:grpSpPr>
         <a:xfrm>
           <a:off x="653597" y="0"/>
-          <a:ext cx="10290628" cy="8019886"/>
+          <a:ext cx="10722428" cy="7816686"/>
           <a:chOff x="529772" y="130628"/>
           <a:chExt cx="6827054" cy="5283472"/>
         </a:xfrm>
@@ -1688,13 +1795,13 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="4" width="18.5703125" customWidth="1"/>
+    <col min="2" max="4" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="21" t="s">
         <v>54</v>
       </c>
@@ -1705,7 +1812,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="23" t="s">
         <v>57</v>
       </c>
@@ -1716,7 +1823,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="23" t="s">
         <v>60</v>
       </c>
@@ -1727,7 +1834,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="23" t="s">
         <v>63</v>
       </c>
@@ -1738,7 +1845,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="23" t="s">
         <v>66</v>
       </c>
@@ -1749,7 +1856,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="23"/>
       <c r="C8" s="24" t="s">
         <v>68</v>
@@ -1758,7 +1865,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="23"/>
       <c r="C9" s="24" t="s">
         <v>69</v>
@@ -1767,7 +1874,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
         <v>70</v>
@@ -1776,35 +1883,35 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="23"/>
       <c r="C11" s="24"/>
       <c r="D11" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="23"/>
       <c r="C13" s="24"/>
       <c r="D13" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B14" s="23"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="23"/>
       <c r="C15" s="24"/>
       <c r="D15" s="24" t="s">
@@ -1825,150 +1932,150 @@
       <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" style="9" customWidth="1"/>
-    <col min="3" max="6" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" style="9" customWidth="1"/>
+    <col min="3" max="6" width="10.54296875" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="25.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.81640625" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="43.5703125" customWidth="1"/>
-    <col min="16" max="16" width="45.5703125" customWidth="1"/>
-    <col min="17" max="17" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.42578125" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="43.54296875" customWidth="1"/>
+    <col min="16" max="16" width="45.54296875" customWidth="1"/>
+    <col min="17" max="17" width="53.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.453125" customWidth="1"/>
+    <col min="20" max="20" width="12.81640625" customWidth="1"/>
     <col min="21" max="22" width="13" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="20.54296875" style="2" customWidth="1"/>
     <col min="24" max="24" width="24" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
+    <col min="25" max="25" width="15.81640625" customWidth="1"/>
     <col min="26" max="26" width="15" customWidth="1"/>
-    <col min="27" max="27" width="10.5703125" customWidth="1"/>
+    <col min="27" max="27" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+    <row r="32" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42" t="s">
+      <c r="D32" s="42"/>
+      <c r="E32" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="46" t="s">
+      <c r="F32" s="47"/>
+      <c r="G32" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="37" t="s">
+      <c r="H32" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="37"/>
+      <c r="I32" s="43"/>
       <c r="L32" s="2"/>
       <c r="M32" s="1"/>
       <c r="W32"/>
       <c r="X32"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" s="45"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
       <c r="L33" s="2"/>
       <c r="M33" s="1"/>
       <c r="W33"/>
       <c r="X33"/>
     </row>
-    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>1</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="50"/>
-      <c r="F34" s="50"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
       <c r="G34" s="19"/>
-      <c r="H34" s="50"/>
-      <c r="I34" s="50"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
       <c r="L34" s="2"/>
       <c r="M34" s="1"/>
       <c r="W34"/>
       <c r="X34"/>
     </row>
-    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>2</v>
       </c>
       <c r="B35" s="15"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="10"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
       <c r="W35"/>
       <c r="X35"/>
     </row>
-    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>3</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
       <c r="L36" s="2"/>
       <c r="M36" s="1"/>
       <c r="W36"/>
       <c r="X36"/>
     </row>
-    <row r="37" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>4</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
-      <c r="E37" s="48"/>
-      <c r="F37" s="49"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="19"/>
-      <c r="H37" s="48"/>
-      <c r="I37" s="49"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="39"/>
       <c r="L37" s="2"/>
       <c r="M37" s="1"/>
       <c r="W37"/>
       <c r="X37"/>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>16</v>
       </c>
@@ -1978,7 +2085,7 @@
       <c r="W39"/>
       <c r="X39"/>
     </row>
-    <row r="40" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
@@ -2003,10 +2110,10 @@
       <c r="H40" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="40" t="s">
+      <c r="I40" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="J40" s="41"/>
+      <c r="J40" s="42"/>
       <c r="K40" s="12" t="s">
         <v>38</v>
       </c>
@@ -2018,7 +2125,7 @@
       <c r="W40"/>
       <c r="X40"/>
     </row>
-    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>1</v>
       </c>
@@ -2029,8 +2136,8 @@
       <c r="F41" s="8"/>
       <c r="G41" s="3"/>
       <c r="H41" s="5"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="49"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
       <c r="K41" s="5"/>
       <c r="L41" s="11"/>
       <c r="R41" s="2"/>
@@ -2038,7 +2145,7 @@
       <c r="W41"/>
       <c r="X41"/>
     </row>
-    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>2</v>
       </c>
@@ -2049,8 +2156,8 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="5"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="49"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
       <c r="K42" s="5"/>
       <c r="L42" s="11"/>
       <c r="R42" s="2"/>
@@ -2058,7 +2165,7 @@
       <c r="W42"/>
       <c r="X42"/>
     </row>
-    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>3</v>
       </c>
@@ -2069,8 +2176,8 @@
       <c r="F43" s="8"/>
       <c r="G43" s="14"/>
       <c r="H43" s="5"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
       <c r="K43" s="5"/>
       <c r="L43" s="11"/>
       <c r="R43" s="2"/>
@@ -2078,7 +2185,7 @@
       <c r="W43"/>
       <c r="X43"/>
     </row>
-    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>4</v>
       </c>
@@ -2089,8 +2196,8 @@
       <c r="F44" s="8"/>
       <c r="G44" s="14"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="49"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
       <c r="K44" s="5"/>
       <c r="L44" s="11"/>
       <c r="R44" s="2"/>
@@ -2098,7 +2205,7 @@
       <c r="W44"/>
       <c r="X44"/>
     </row>
-    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>5</v>
       </c>
@@ -2109,8 +2216,8 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="48"/>
-      <c r="J45" s="49"/>
+      <c r="I45" s="38"/>
+      <c r="J45" s="39"/>
       <c r="K45" s="5"/>
       <c r="L45" s="11"/>
       <c r="P45" s="2"/>
@@ -2118,7 +2225,7 @@
       <c r="W45"/>
       <c r="X45"/>
     </row>
-    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>6</v>
       </c>
@@ -2129,8 +2236,8 @@
       <c r="F46" s="3"/>
       <c r="G46" s="18"/>
       <c r="H46" s="5"/>
-      <c r="I46" s="48"/>
-      <c r="J46" s="49"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="39"/>
       <c r="K46" s="5"/>
       <c r="L46" s="11"/>
       <c r="P46" s="2"/>
@@ -2138,7 +2245,7 @@
       <c r="W46"/>
       <c r="X46"/>
     </row>
-    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>7</v>
       </c>
@@ -2149,8 +2256,8 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="5"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="49"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="39"/>
       <c r="K47" s="5"/>
       <c r="L47" s="11"/>
       <c r="P47" s="2"/>
@@ -2158,7 +2265,7 @@
       <c r="W47"/>
       <c r="X47"/>
     </row>
-    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>8</v>
       </c>
@@ -2169,8 +2276,8 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="5"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="49"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="39"/>
       <c r="K48" s="5"/>
       <c r="L48" s="11"/>
       <c r="P48" s="2"/>
@@ -2178,7 +2285,7 @@
       <c r="W48"/>
       <c r="X48"/>
     </row>
-    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>9</v>
       </c>
@@ -2189,8 +2296,8 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="49"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="39"/>
       <c r="K49" s="5"/>
       <c r="L49" s="11"/>
       <c r="P49" s="2"/>
@@ -2198,7 +2305,7 @@
       <c r="W49"/>
       <c r="X49"/>
     </row>
-    <row r="50" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>10</v>
       </c>
@@ -2209,8 +2316,8 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="5"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="49"/>
+      <c r="I50" s="38"/>
+      <c r="J50" s="39"/>
       <c r="K50" s="5"/>
       <c r="L50" s="11"/>
       <c r="P50" s="2"/>
@@ -2218,37 +2325,38 @@
       <c r="W50"/>
       <c r="X50"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M51" s="2"/>
       <c r="N51" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M53" s="2"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M54" s="2"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M55" s="2"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M56" s="2"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M57" s="2"/>
       <c r="N57" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I46:J46"/>
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I48:J48"/>
-    <mergeCell ref="I49:J49"/>
-    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
     <mergeCell ref="I45:J45"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="H34:I34"/>
@@ -2263,12 +2371,11 @@
     <mergeCell ref="I44:J44"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H32:I33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="I50:J50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2279,232 +2386,235 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A31:Z58"/>
+  <dimension ref="A31:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" style="9" customWidth="1"/>
-    <col min="3" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" style="9" customWidth="1"/>
+    <col min="3" max="5" width="10.54296875" style="30" customWidth="1"/>
+    <col min="6" max="6" width="10.54296875" customWidth="1"/>
+    <col min="7" max="7" width="35.26953125" customWidth="1"/>
     <col min="8" max="9" width="14" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20.85546875" style="35" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="52.85546875" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="11" max="11" width="25.453125" customWidth="1"/>
+    <col min="12" max="12" width="11.81640625" customWidth="1"/>
+    <col min="13" max="13" width="20.81640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.36328125" customWidth="1"/>
+    <col min="15" max="15" width="14.81640625" customWidth="1"/>
     <col min="16" max="16" width="10" customWidth="1"/>
-    <col min="17" max="17" width="43.5703125" customWidth="1"/>
-    <col min="18" max="18" width="45.5703125" customWidth="1"/>
-    <col min="19" max="19" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="12.42578125" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="43.54296875" customWidth="1"/>
+    <col min="18" max="18" width="45.54296875" customWidth="1"/>
+    <col min="19" max="19" width="53.81640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="12.453125" customWidth="1"/>
+    <col min="22" max="22" width="12.81640625" customWidth="1"/>
     <col min="23" max="24" width="13" customWidth="1"/>
-    <col min="25" max="25" width="20.5703125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="20.54296875" style="2" customWidth="1"/>
     <col min="26" max="26" width="24" style="1" customWidth="1"/>
-    <col min="27" max="27" width="15.85546875" customWidth="1"/>
+    <col min="27" max="27" width="15.81640625" customWidth="1"/>
     <col min="28" max="28" width="15" customWidth="1"/>
-    <col min="29" max="29" width="10.5703125" customWidth="1"/>
+    <col min="29" max="29" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+    <row r="32" spans="1:26" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42" t="s">
+      <c r="D32" s="42"/>
+      <c r="E32" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="46" t="s">
+      <c r="F32" s="47"/>
+      <c r="G32" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="42" t="s">
+      <c r="H32" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="43"/>
+      <c r="I32" s="47"/>
       <c r="N32" s="2"/>
       <c r="O32" s="1"/>
       <c r="Y32"/>
       <c r="Z32"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A33" s="45"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="44"/>
-      <c r="I33" s="45"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="48"/>
+      <c r="I33" s="49"/>
       <c r="N33" s="2"/>
       <c r="O33" s="1"/>
       <c r="Y33"/>
       <c r="Z33"/>
     </row>
-    <row r="34" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>1</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="31">
         <v>2</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="31">
         <v>2</v>
       </c>
-      <c r="E34" s="50" t="s">
-        <v>87</v>
-      </c>
-      <c r="F34" s="50"/>
+      <c r="E34" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" s="40"/>
       <c r="G34" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H34" s="53" t="s">
+      <c r="H34" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="I34" s="54"/>
+      <c r="I34" s="55"/>
       <c r="N34" s="2"/>
       <c r="O34" s="1"/>
       <c r="Y34"/>
       <c r="Z34"/>
     </row>
-    <row r="35" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>2</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="31">
         <v>1</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="31">
         <v>2</v>
       </c>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="F35" s="40"/>
+      <c r="G35" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="F35" s="50"/>
-      <c r="G35" s="10" t="s">
+      <c r="H35" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="H35" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="I35" s="54"/>
+      <c r="I35" s="55"/>
       <c r="N35" s="2"/>
       <c r="O35" s="1"/>
       <c r="Y35"/>
       <c r="Z35"/>
     </row>
-    <row r="36" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>3</v>
       </c>
       <c r="B36" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="31">
+        <v>1</v>
+      </c>
+      <c r="D36" s="31">
+        <v>2</v>
+      </c>
+      <c r="E36" s="40" t="str">
+        <f>E35</f>
+        <v>angle block or surface plate on flat face of part</v>
+      </c>
+      <c r="F36" s="40"/>
+      <c r="G36" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H36" s="54" t="s">
         <v>86</v>
       </c>
-      <c r="C36" s="5">
-        <v>1</v>
-      </c>
-      <c r="D36" s="5">
-        <v>2</v>
-      </c>
-      <c r="E36" s="50" t="s">
-        <v>83</v>
-      </c>
-      <c r="F36" s="50"/>
-      <c r="G36" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H36" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="I36" s="54"/>
+      <c r="I36" s="55"/>
       <c r="N36" s="2"/>
       <c r="O36" s="1"/>
       <c r="Y36"/>
       <c r="Z36"/>
     </row>
-    <row r="37" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>4</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="C37" s="5">
+        <v>87</v>
+      </c>
+      <c r="C37" s="31">
         <v>1</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="31">
         <v>2</v>
       </c>
-      <c r="E37" s="48" t="s">
+      <c r="E37" s="40" t="str">
+        <f>E36</f>
+        <v>angle block or surface plate on flat face of part</v>
+      </c>
+      <c r="F37" s="40"/>
+      <c r="G37" s="19" t="s">
         <v>83</v>
       </c>
-      <c r="F37" s="49"/>
-      <c r="G37" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="H37" s="53" t="s">
-        <v>90</v>
-      </c>
-      <c r="I37" s="54"/>
+      <c r="H37" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="I37" s="55"/>
       <c r="N37" s="2"/>
       <c r="O37" s="1"/>
       <c r="Y37"/>
       <c r="Z37"/>
     </row>
-    <row r="39" spans="1:26" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>16</v>
       </c>
       <c r="B39" s="12"/>
-      <c r="I39" s="40" t="s">
+      <c r="I39" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="J39" s="41"/>
+      <c r="J39" s="42"/>
       <c r="V39" s="2"/>
       <c r="W39" s="1"/>
       <c r="Y39"/>
       <c r="Z39"/>
     </row>
-    <row r="40" spans="1:26" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B40" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E40" s="32" t="s">
         <v>36</v>
       </c>
       <c r="F40" s="12" t="s">
@@ -2522,10 +2632,10 @@
       <c r="J40" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="40" t="s">
+      <c r="K40" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="L40" s="41"/>
+      <c r="L40" s="42"/>
       <c r="M40" s="27" t="s">
         <v>38</v>
       </c>
@@ -2537,138 +2647,139 @@
       <c r="Y40"/>
       <c r="Z40"/>
     </row>
-    <row r="41" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>1</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="C41" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="D41" s="56">
+        <v>89</v>
+      </c>
+      <c r="C41" s="56">
+        <v>2</v>
+      </c>
+      <c r="D41" s="37">
         <v>2E-3</v>
       </c>
-      <c r="E41" s="56">
+      <c r="E41" s="37">
         <f>E43-D41</f>
         <v>0.37424999999999997</v>
       </c>
-      <c r="F41" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="G41" s="57" t="s">
+      <c r="F41" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G41" s="37" t="s">
+        <v>105</v>
+      </c>
+      <c r="H41" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H41" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="I41" s="3">
+      <c r="I41" s="5">
         <v>2</v>
       </c>
       <c r="J41" s="5">
-        <v>2</v>
-      </c>
-      <c r="K41" s="48" t="s">
-        <v>92</v>
-      </c>
-      <c r="L41" s="49"/>
-      <c r="M41" s="36" t="s">
-        <v>93</v>
-      </c>
-      <c r="N41" s="51" t="s">
-        <v>98</v>
+        <v>3</v>
+      </c>
+      <c r="K41" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="L41" s="39"/>
+      <c r="M41" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="N41" s="52" t="s">
+        <v>96</v>
       </c>
       <c r="T41" s="2"/>
       <c r="U41" s="1"/>
       <c r="Y41"/>
       <c r="Z41"/>
     </row>
-    <row r="42" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <f>A41+1</f>
         <v>2</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C42" s="55" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="56">
+        <v>92</v>
+      </c>
+      <c r="C42" s="56">
+        <v>3.5</v>
+      </c>
+      <c r="D42" s="37">
         <v>0.1</v>
       </c>
-      <c r="E42" s="56">
+      <c r="E42" s="37">
         <f>E43-D42</f>
         <v>0.27625</v>
       </c>
-      <c r="F42" s="56" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="57" t="str">
+      <c r="F42" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G42" s="37" t="str">
         <f>G41</f>
-        <v>Height Gage, or a functional gage with a pin in the hole and the extension of the pin must fit in a slot</v>
-      </c>
-      <c r="H42" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="I42" s="3">
+        <v>Gage pin + Height Gage, or a functional gage with a pin in the hole and the extension of the pin must fit in a slot</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I42" s="5">
         <v>2</v>
       </c>
       <c r="J42" s="5">
-        <v>2</v>
-      </c>
-      <c r="K42" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="L42" s="49"/>
-      <c r="M42" s="36" t="str">
+        <v>3</v>
+      </c>
+      <c r="K42" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="L42" s="39"/>
+      <c r="M42" s="31" t="str">
         <f>M41</f>
         <v>no, it is the void at the center of a hole.</v>
       </c>
-      <c r="N42" s="52"/>
+      <c r="N42" s="53"/>
       <c r="T42" s="2"/>
       <c r="U42" s="1"/>
       <c r="Y42"/>
       <c r="Z42"/>
     </row>
-    <row r="43" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
-        <f t="shared" ref="A43:A56" si="0">A42+1</f>
+        <f t="shared" ref="A43:A59" si="0">A42+1</f>
         <v>3</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C43" s="55">
+        <v>93</v>
+      </c>
+      <c r="C43" s="56">
         <v>0.377</v>
       </c>
-      <c r="D43" s="56">
+      <c r="D43" s="37">
         <f>-F43+E43</f>
         <v>1.3499999999999623E-3</v>
       </c>
-      <c r="E43" s="55">
+      <c r="E43" s="56">
         <v>0.37624999999999997</v>
       </c>
-      <c r="F43" s="34">
+      <c r="F43" s="29">
         <v>0.37490000000000001</v>
       </c>
-      <c r="G43" s="57" t="s">
-        <v>96</v>
-      </c>
-      <c r="H43" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="I43" s="14"/>
+      <c r="G43" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I43" s="5"/>
       <c r="J43" s="5"/>
-      <c r="K43" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="L43" s="49"/>
-      <c r="M43" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="N43" s="30" t="s">
+      <c r="K43" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="L43" s="39"/>
+      <c r="M43" s="31" t="str">
+        <f>M44</f>
+        <v>yes, it's the size of a hole</v>
+      </c>
+      <c r="N43" s="28" t="s">
         <v>47</v>
       </c>
       <c r="T43" s="2"/>
@@ -2676,46 +2787,46 @@
       <c r="Y43"/>
       <c r="Z43"/>
     </row>
-    <row r="44" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>101</v>
-      </c>
-      <c r="C44" s="55">
+        <v>98</v>
+      </c>
+      <c r="C44" s="56">
         <v>0.159</v>
       </c>
-      <c r="D44" s="56">
+      <c r="D44" s="37">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E44" s="55">
+      <c r="E44" s="56">
         <f>C44-D44</f>
         <v>0.154</v>
       </c>
-      <c r="F44" s="55">
+      <c r="F44" s="35">
         <f>C44+D44</f>
         <v>0.16400000000000001</v>
       </c>
-      <c r="G44" s="57" t="str">
+      <c r="G44" s="37" t="str">
         <f>G43</f>
         <v>go/nogo</v>
       </c>
-      <c r="H44" s="32" t="str">
+      <c r="H44" s="5" t="str">
         <f>H43</f>
         <v>NA</v>
       </c>
-      <c r="I44" s="14"/>
+      <c r="I44" s="5"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="48" t="str">
+      <c r="K44" s="38" t="str">
         <f>K43</f>
         <v>NA</v>
       </c>
-      <c r="L44" s="49"/>
-      <c r="M44" s="36" t="str">
-        <f>M43</f>
-        <v>yes</v>
+      <c r="L44" s="39"/>
+      <c r="M44" s="31" t="str">
+        <f>M46</f>
+        <v>yes, it's the size of a hole</v>
       </c>
       <c r="N44" s="11" t="str">
         <f>N43</f>
@@ -2726,322 +2837,779 @@
       <c r="Y44"/>
       <c r="Z44"/>
     </row>
-    <row r="45" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="C45" s="55" t="str">
-        <f>C42</f>
-        <v>NA</v>
-      </c>
-      <c r="D45" s="56">
+        <v>97</v>
+      </c>
+      <c r="C45" s="56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D45" s="37">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="E45" s="56">
+      <c r="E45" s="37">
         <f>E44-D45</f>
         <v>0.14899999999999999</v>
       </c>
-      <c r="F45" s="56" t="str">
+      <c r="F45" s="36" t="str">
         <f>F42</f>
         <v>NA</v>
       </c>
-      <c r="G45" s="57" t="s">
-        <v>102</v>
-      </c>
-      <c r="H45" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="I45" s="3">
+      <c r="G45" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I45" s="5">
         <v>3</v>
       </c>
       <c r="J45" s="5">
         <v>3</v>
       </c>
-      <c r="K45" s="48" t="s">
-        <v>103</v>
-      </c>
-      <c r="L45" s="49"/>
-      <c r="M45" s="36" t="str">
+      <c r="K45" s="38" t="s">
+        <v>112</v>
+      </c>
+      <c r="L45" s="39"/>
+      <c r="M45" s="31" t="str">
         <f>M42</f>
         <v>no, it is the void at the center of a hole.</v>
       </c>
-      <c r="N45" s="30" t="str">
-        <f>"The axis of the feature must fall within a cylindrical tolerance zone with a diameter of "&amp;D45&amp;".  The zone will be located relative to the Datums by the basic dimensions."</f>
-        <v>The axis of the feature must fall within a cylindrical tolerance zone with a diameter of 0.005.  The zone will be located relative to the Datums by the basic dimensions.</v>
+      <c r="N45" s="28" t="str">
+        <f>"The axis of the feature must fall within a circular tolerance zone with a diameter of "&amp;D45&amp;" on the surface opposite datum C (because of the (P) 0  ).  The zone will be located relative to the Datums by the basic dimensions."</f>
+        <v>The axis of the feature must fall within a circular tolerance zone with a diameter of 0.005 on the surface opposite datum C (because of the (P) 0  ).  The zone will be located relative to the Datums by the basic dimensions.</v>
       </c>
       <c r="R45" s="2"/>
       <c r="S45" s="1"/>
       <c r="Y45"/>
       <c r="Z45"/>
     </row>
-    <row r="46" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="55"/>
-      <c r="D46" s="56"/>
-      <c r="E46" s="56"/>
-      <c r="F46" s="56"/>
-      <c r="G46" s="57"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="18"/>
+      <c r="B46" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="C46" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="D46" s="37" t="str">
+        <f>C46</f>
+        <v>NA (threaded)</v>
+      </c>
+      <c r="E46" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G46" s="37" t="s">
+        <v>106</v>
+      </c>
+      <c r="H46" s="5" t="str">
+        <f>H55</f>
+        <v>NA</v>
+      </c>
+      <c r="I46" s="5"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="49"/>
-      <c r="M46" s="36"/>
-      <c r="N46" s="11"/>
+      <c r="K46" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="L46" s="39"/>
+      <c r="M46" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="N46" s="34" t="s">
+        <v>108</v>
+      </c>
       <c r="R46" s="2"/>
       <c r="S46" s="1"/>
       <c r="Y46"/>
       <c r="Z46"/>
     </row>
-    <row r="47" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B47" s="16"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="56"/>
-      <c r="E47" s="56"/>
-      <c r="F47" s="56"/>
-      <c r="G47" s="57"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="5"/>
-      <c r="K47" s="28"/>
-      <c r="L47" s="29"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="30"/>
-      <c r="R47" s="2"/>
-      <c r="S47" s="1"/>
+      <c r="B47" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="D47" s="37">
+        <v>2E-3</v>
+      </c>
+      <c r="E47" s="37" t="str">
+        <f>E56</f>
+        <v>NA</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I47" s="5">
+        <v>3</v>
+      </c>
+      <c r="J47" s="5">
+        <v>3</v>
+      </c>
+      <c r="K47" s="38" t="s">
+        <v>107</v>
+      </c>
+      <c r="L47" s="39"/>
+      <c r="M47" s="31" t="str">
+        <f>M45</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
+      <c r="N47" s="34" t="str">
+        <f>"The axis of the feature must fall within a circular tolerance zone with a diameter of "&amp;D47&amp;" on the surface opposite datum C (because of the (P) 0  ).  The zone will be located relative to the Datums by the basic dimensions."</f>
+        <v>The axis of the feature must fall within a circular tolerance zone with a diameter of 0.002 on the surface opposite datum C (because of the (P) 0  ).  The zone will be located relative to the Datums by the basic dimensions.</v>
+      </c>
+      <c r="T47" s="2"/>
+      <c r="U47" s="1"/>
       <c r="Y47"/>
       <c r="Z47"/>
     </row>
-    <row r="48" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="55"/>
-      <c r="D48" s="56"/>
-      <c r="E48" s="56"/>
-      <c r="F48" s="56"/>
-      <c r="G48" s="57"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="5"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="29"/>
-      <c r="M48" s="36"/>
-      <c r="N48" s="30"/>
+      <c r="B48" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C48" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="E48" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G48" s="37" t="s">
+        <v>115</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I48" s="5">
+        <v>1</v>
+      </c>
+      <c r="J48" s="5">
+        <v>2</v>
+      </c>
+      <c r="K48" s="38" t="s">
+        <v>120</v>
+      </c>
+      <c r="L48" s="39"/>
+      <c r="M48" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="N48" s="34" t="s">
+        <v>117</v>
+      </c>
       <c r="R48" s="2"/>
       <c r="S48" s="1"/>
       <c r="Y48"/>
       <c r="Z48"/>
     </row>
-    <row r="49" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B49" s="16"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="56"/>
-      <c r="E49" s="56"/>
-      <c r="F49" s="56"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="29"/>
-      <c r="M49" s="36"/>
-      <c r="N49" s="30"/>
+      <c r="B49" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C49" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="E49" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F49" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="H49" s="5" t="str">
+        <f>H48</f>
+        <v>A, C</v>
+      </c>
+      <c r="I49" s="5">
+        <v>1</v>
+      </c>
+      <c r="J49" s="5">
+        <v>2</v>
+      </c>
+      <c r="K49" s="38" t="str">
+        <f>K48</f>
+        <v>The vertical angle of this hole affects the vertical ovalness of the end of the hole, which needs to be controlled to affect the range along the vertical axis where exhausting can occur.</v>
+      </c>
+      <c r="L49" s="39"/>
+      <c r="M49" s="31" t="str">
+        <f>M48</f>
+        <v>no, it is a single surface</v>
+      </c>
+      <c r="N49" s="34" t="str">
+        <f>N48</f>
+        <v>the space between two parallel planes, perpendicular to datum C and parallel to datum A, 0.05 in apart, the 0.5 in long axis of this hole must be between them</v>
+      </c>
       <c r="R49" s="2"/>
       <c r="S49" s="1"/>
       <c r="Y49"/>
       <c r="Z49"/>
     </row>
-    <row r="50" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="55"/>
-      <c r="D50" s="56"/>
-      <c r="E50" s="56"/>
-      <c r="F50" s="56"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="18"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="28"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="36"/>
-      <c r="N50" s="30"/>
+      <c r="B50" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C50" s="56">
+        <v>0.19350000000000001</v>
+      </c>
+      <c r="D50" s="56">
+        <f>E50-F50</f>
+        <v>-5.6999999999999829E-3</v>
+      </c>
+      <c r="E50" s="56">
+        <f>0.19+5/1000</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="F50" s="56">
+        <f>0.19+10.7/1000</f>
+        <v>0.20069999999999999</v>
+      </c>
+      <c r="G50" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="H50" s="56" t="str">
+        <f>H55</f>
+        <v>NA</v>
+      </c>
+      <c r="I50" s="56"/>
+      <c r="J50" s="56"/>
+      <c r="K50" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="L50" s="39"/>
+      <c r="M50" s="31" t="str">
+        <f>M46</f>
+        <v>yes, it's the size of a hole</v>
+      </c>
+      <c r="N50" s="34" t="s">
+        <v>142</v>
+      </c>
       <c r="R50" s="2"/>
       <c r="S50" s="1"/>
       <c r="Y50"/>
       <c r="Z50"/>
     </row>
-    <row r="51" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B51" s="16"/>
-      <c r="C51" s="55"/>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
-      <c r="F51" s="56"/>
-      <c r="G51" s="57"/>
-      <c r="H51" s="33"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="5"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="29"/>
-      <c r="M51" s="36"/>
-      <c r="N51" s="30"/>
+      <c r="B51" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C51" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="37">
+        <v>2E-3</v>
+      </c>
+      <c r="E51" s="37">
+        <f>E50-D51</f>
+        <v>0.193</v>
+      </c>
+      <c r="F51" s="36" t="str">
+        <f>F47</f>
+        <v>NA</v>
+      </c>
+      <c r="G51" s="36" t="str">
+        <f>G47</f>
+        <v>thread gage + height gage</v>
+      </c>
+      <c r="H51" s="36" t="s">
+        <v>101</v>
+      </c>
+      <c r="I51" s="36">
+        <f>I47</f>
+        <v>3</v>
+      </c>
+      <c r="J51" s="36">
+        <f>J47</f>
+        <v>3</v>
+      </c>
+      <c r="K51" s="38" t="s">
+        <v>121</v>
+      </c>
+      <c r="L51" s="39"/>
+      <c r="M51" s="31" t="str">
+        <f>M47</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
+      <c r="N51" s="34" t="str">
+        <f>"The axis of the feature must fall within a circular tolerance zone with a diameter of "&amp;D51&amp;" on the surface opposite datum C (because of the (P) 0  ).  The zone will be located relative to the Datums by the basic dimensions."</f>
+        <v>The axis of the feature must fall within a circular tolerance zone with a diameter of 0.002 on the surface opposite datum C (because of the (P) 0  ).  The zone will be located relative to the Datums by the basic dimensions.</v>
+      </c>
       <c r="R51" s="2"/>
       <c r="S51" s="1"/>
       <c r="Y51"/>
       <c r="Z51"/>
     </row>
-    <row r="52" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B52" s="16"/>
-      <c r="C52" s="55"/>
-      <c r="D52" s="56"/>
-      <c r="E52" s="56"/>
-      <c r="F52" s="56"/>
-      <c r="G52" s="57"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="18"/>
-      <c r="J52" s="5"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="29"/>
-      <c r="M52" s="36"/>
-      <c r="N52" s="30"/>
+      <c r="B52" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="E52" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F52" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G52" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I52" s="5">
+        <v>1</v>
+      </c>
+      <c r="J52" s="5">
+        <v>2</v>
+      </c>
+      <c r="K52" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="L52" s="39"/>
+      <c r="M52" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="N52" s="34" t="s">
+        <v>127</v>
+      </c>
       <c r="R52" s="2"/>
       <c r="S52" s="1"/>
       <c r="Y52"/>
       <c r="Z52"/>
     </row>
-    <row r="53" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B53" s="16"/>
-      <c r="C53" s="55"/>
-      <c r="D53" s="56"/>
-      <c r="E53" s="56"/>
-      <c r="F53" s="56"/>
-      <c r="G53" s="57"/>
-      <c r="H53" s="33"/>
-      <c r="I53" s="18"/>
-      <c r="J53" s="5"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="29"/>
-      <c r="M53" s="36"/>
-      <c r="N53" s="30"/>
+      <c r="B53" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="56" t="str">
+        <f>C52</f>
+        <v>NA</v>
+      </c>
+      <c r="D53" s="56">
+        <v>0.15</v>
+      </c>
+      <c r="E53" s="56" t="str">
+        <f t="shared" ref="D53:J53" si="1">E52</f>
+        <v>NA</v>
+      </c>
+      <c r="F53" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>NA</v>
+      </c>
+      <c r="G53" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>dial indicator</v>
+      </c>
+      <c r="H53" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>C</v>
+      </c>
+      <c r="I53" s="56">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J53" s="56">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K53" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="L53" s="39"/>
+      <c r="M53" s="31" t="str">
+        <f>M52</f>
+        <v>no, it is a surface.</v>
+      </c>
+      <c r="N53" s="34" t="s">
+        <v>130</v>
+      </c>
       <c r="R53" s="2"/>
       <c r="S53" s="1"/>
       <c r="Y53"/>
       <c r="Z53"/>
     </row>
-    <row r="54" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B54" s="16"/>
-      <c r="C54" s="55"/>
-      <c r="D54" s="56"/>
-      <c r="E54" s="56"/>
-      <c r="F54" s="56"/>
-      <c r="G54" s="57"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="18"/>
-      <c r="J54" s="5"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="29"/>
-      <c r="M54" s="36"/>
-      <c r="N54" s="30"/>
+      <c r="B54" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="37">
+        <v>1E-3</v>
+      </c>
+      <c r="E54" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F54" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G54" s="37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1</v>
+      </c>
+      <c r="J54" s="5">
+        <v>2</v>
+      </c>
+      <c r="K54" s="38" t="s">
+        <v>132</v>
+      </c>
+      <c r="L54" s="39"/>
+      <c r="M54" s="31" t="str">
+        <f>M53</f>
+        <v>no, it is a surface.</v>
+      </c>
+      <c r="N54" s="34" t="s">
+        <v>133</v>
+      </c>
       <c r="R54" s="2"/>
       <c r="S54" s="1"/>
       <c r="Y54"/>
       <c r="Z54"/>
     </row>
-    <row r="55" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B55" s="16"/>
-      <c r="C55" s="55"/>
-      <c r="D55" s="56"/>
-      <c r="E55" s="56"/>
-      <c r="F55" s="56"/>
-      <c r="G55" s="57"/>
-      <c r="H55" s="33"/>
-      <c r="I55" s="18"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="28"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="36"/>
-      <c r="N55" s="30"/>
+      <c r="B55" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" s="56" t="str">
+        <f>C46</f>
+        <v>NA (threaded)</v>
+      </c>
+      <c r="D55" s="56" t="str">
+        <f t="shared" ref="D55:N55" si="2">D46</f>
+        <v>NA (threaded)</v>
+      </c>
+      <c r="E55" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="G55" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>thread gage</v>
+      </c>
+      <c r="H55" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="I55" s="56"/>
+      <c r="J55" s="56"/>
+      <c r="K55" s="38" t="str">
+        <f t="shared" si="2"/>
+        <v>NA</v>
+      </c>
+      <c r="L55" s="39">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>yes, it's the size of a hole</v>
+      </c>
+      <c r="N55" s="56" t="str">
+        <f t="shared" si="2"/>
+        <v>the shape of thread gage must fit inside the threaded hole and not wiggle too much</v>
+      </c>
       <c r="R55" s="2"/>
       <c r="S55" s="1"/>
       <c r="Y55"/>
       <c r="Z55"/>
     </row>
-    <row r="56" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B56" s="16"/>
-      <c r="C56" s="55"/>
-      <c r="D56" s="56"/>
-      <c r="E56" s="56"/>
-      <c r="F56" s="56"/>
-      <c r="G56" s="57"/>
-      <c r="H56" s="33"/>
-      <c r="I56" s="18"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="28"/>
-      <c r="L56" s="29"/>
-      <c r="M56" s="36"/>
-      <c r="N56" s="30"/>
+      <c r="B56" s="16" t="str">
+        <f>"Threaded hole for baseplate bolt position to "&amp;H56</f>
+        <v>Threaded hole for baseplate bolt position to C</v>
+      </c>
+      <c r="C56" s="56">
+        <v>0.25</v>
+      </c>
+      <c r="D56" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="E56" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G56" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="I56" s="5">
+        <v>1</v>
+      </c>
+      <c r="J56" s="5">
+        <v>2</v>
+      </c>
+      <c r="K56" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="L56" s="39"/>
+      <c r="M56" s="31" t="str">
+        <f>M51</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
+      <c r="N56" s="52" t="s">
+        <v>147</v>
+      </c>
       <c r="R56" s="2"/>
       <c r="S56" s="1"/>
       <c r="Y56"/>
       <c r="Z56"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O57" s="2"/>
-      <c r="P57" s="1"/>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="O58" s="2"/>
-      <c r="P58" s="1"/>
+    <row r="57" spans="1:26" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B57" s="16" t="str">
+        <f>"Threaded hole for baseplate bolt position to "&amp;H57</f>
+        <v>Threaded hole for baseplate bolt position to C, D</v>
+      </c>
+      <c r="C57" s="56" t="str">
+        <f>"0.75, "&amp;(3.5+0.75)</f>
+        <v>0.75, 4.25</v>
+      </c>
+      <c r="D57" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="E57" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F57" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="37" t="str">
+        <f>G56</f>
+        <v>thread gage + height gage</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I57" s="5">
+        <v>2</v>
+      </c>
+      <c r="J57" s="5">
+        <v>3</v>
+      </c>
+      <c r="K57" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="L57" s="39"/>
+      <c r="M57" s="31" t="str">
+        <f>M56</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
+      <c r="N57" s="53"/>
+      <c r="R57" s="2"/>
+      <c r="S57" s="1"/>
+      <c r="Y57"/>
+      <c r="Z57"/>
+    </row>
+    <row r="58" spans="1:26" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C58" s="56">
+        <v>3.5</v>
+      </c>
+      <c r="D58" s="37">
+        <v>2E-3</v>
+      </c>
+      <c r="E58" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F58" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G58" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="I58" s="5">
+        <v>2</v>
+      </c>
+      <c r="J58" s="5">
+        <v>2</v>
+      </c>
+      <c r="K58" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="L58" s="39"/>
+      <c r="M58" s="31" t="str">
+        <f>M57</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
+      <c r="N58" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="R58" s="2"/>
+      <c r="S58" s="1"/>
+      <c r="Y58"/>
+      <c r="Z58"/>
+    </row>
+    <row r="59" spans="1:26" ht="41" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="4">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="C59" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="37">
+        <v>2E-3</v>
+      </c>
+      <c r="E59" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="G59" s="37" t="str">
+        <f>G57</f>
+        <v>thread gage + height gage</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I59" s="5">
+        <v>2</v>
+      </c>
+      <c r="J59" s="5">
+        <v>3</v>
+      </c>
+      <c r="K59" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="L59" s="39"/>
+      <c r="M59" s="31" t="str">
+        <f>M58</f>
+        <v>no, it is the void at the center of a hole.</v>
+      </c>
+      <c r="N59" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="R59" s="2"/>
+      <c r="S59" s="1"/>
+      <c r="Y59"/>
+      <c r="Z59"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="K46:L46"/>
+  <mergeCells count="37">
+    <mergeCell ref="K58:L58"/>
+    <mergeCell ref="K59:L59"/>
+    <mergeCell ref="N56:N57"/>
+    <mergeCell ref="K53:L53"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="K56:L56"/>
+    <mergeCell ref="K57:L57"/>
+    <mergeCell ref="K48:L48"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="K51:L51"/>
+    <mergeCell ref="K52:L52"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="E32:F33"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="K47:L47"/>
     <mergeCell ref="K45:L45"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
@@ -3051,19 +3619,7 @@
     <mergeCell ref="K42:L42"/>
     <mergeCell ref="K43:L43"/>
     <mergeCell ref="K44:L44"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="H32:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="K46:L46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3080,82 +3636,82 @@
       <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="25.5703125" style="9" customWidth="1"/>
-    <col min="3" max="6" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="25.54296875" style="9" customWidth="1"/>
+    <col min="3" max="6" width="10.54296875" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="11" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="52.85546875" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="25.453125" customWidth="1"/>
+    <col min="10" max="10" width="11.81640625" customWidth="1"/>
+    <col min="11" max="11" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="52.81640625" customWidth="1"/>
+    <col min="13" max="13" width="14.81640625" customWidth="1"/>
     <col min="14" max="14" width="10" customWidth="1"/>
-    <col min="15" max="15" width="43.5703125" customWidth="1"/>
-    <col min="16" max="16" width="45.5703125" customWidth="1"/>
-    <col min="17" max="17" width="53.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.42578125" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="43.54296875" customWidth="1"/>
+    <col min="16" max="16" width="45.54296875" customWidth="1"/>
+    <col min="17" max="17" width="53.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.453125" customWidth="1"/>
+    <col min="20" max="20" width="12.81640625" customWidth="1"/>
     <col min="21" max="22" width="13" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" style="2" customWidth="1"/>
+    <col min="23" max="23" width="20.54296875" style="2" customWidth="1"/>
     <col min="24" max="24" width="24" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" customWidth="1"/>
+    <col min="25" max="25" width="15.81640625" customWidth="1"/>
     <col min="26" max="26" width="15" customWidth="1"/>
-    <col min="27" max="27" width="10.5703125" customWidth="1"/>
+    <col min="27" max="27" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+    <row r="32" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="41"/>
-      <c r="E32" s="42" t="s">
+      <c r="D32" s="42"/>
+      <c r="E32" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F32" s="43"/>
-      <c r="G32" s="46" t="s">
+      <c r="F32" s="47"/>
+      <c r="G32" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="37" t="s">
+      <c r="H32" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="I32" s="37"/>
+      <c r="I32" s="43"/>
       <c r="L32" s="2"/>
       <c r="M32" s="1"/>
       <c r="W32"/>
       <c r="X32"/>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="39"/>
-      <c r="B33" s="39"/>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A33" s="45"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E33" s="44"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="47"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
+      <c r="E33" s="48"/>
+      <c r="F33" s="49"/>
+      <c r="G33" s="51"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
       <c r="L33" s="2"/>
       <c r="M33" s="1"/>
       <c r="W33"/>
       <c r="X33"/>
     </row>
-    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>1</v>
       </c>
@@ -3168,23 +3724,23 @@
       <c r="D34" s="5">
         <v>2</v>
       </c>
-      <c r="E34" s="50" t="s">
+      <c r="E34" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="50"/>
+      <c r="F34" s="40"/>
       <c r="G34" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H34" s="50" t="s">
+      <c r="H34" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="I34" s="50"/>
+      <c r="I34" s="40"/>
       <c r="L34" s="2"/>
       <c r="M34" s="1"/>
       <c r="W34"/>
       <c r="X34"/>
     </row>
-    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>2</v>
       </c>
@@ -3197,23 +3753,23 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="50" t="s">
+      <c r="E35" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="50"/>
+      <c r="F35" s="40"/>
       <c r="G35" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="50" t="s">
+      <c r="H35" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="50"/>
+      <c r="I35" s="40"/>
       <c r="L35" s="2"/>
       <c r="M35" s="1"/>
       <c r="W35"/>
       <c r="X35"/>
     </row>
-    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>3</v>
       </c>
@@ -3226,23 +3782,23 @@
       <c r="D36" s="5">
         <v>0</v>
       </c>
-      <c r="E36" s="50" t="s">
+      <c r="E36" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="50"/>
+      <c r="F36" s="40"/>
       <c r="G36" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H36" s="50" t="s">
+      <c r="H36" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="I36" s="50"/>
+      <c r="I36" s="40"/>
       <c r="L36" s="2"/>
       <c r="M36" s="1"/>
       <c r="W36"/>
       <c r="X36"/>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>16</v>
       </c>
@@ -3252,7 +3808,7 @@
       <c r="W38"/>
       <c r="X38"/>
     </row>
-    <row r="39" spans="1:24" ht="57.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" ht="58" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -3277,10 +3833,10 @@
       <c r="H39" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="I39" s="40" t="s">
+      <c r="I39" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="J39" s="41"/>
+      <c r="J39" s="42"/>
       <c r="K39" s="27" t="s">
         <v>38</v>
       </c>
@@ -3292,7 +3848,7 @@
       <c r="W39"/>
       <c r="X39"/>
     </row>
-    <row r="40" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>1</v>
       </c>
@@ -3317,10 +3873,10 @@
       <c r="H40" s="5">
         <v>0</v>
       </c>
-      <c r="I40" s="48" t="s">
+      <c r="I40" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="J40" s="49"/>
+      <c r="J40" s="39"/>
       <c r="K40" s="5" t="s">
         <v>77</v>
       </c>
@@ -3332,7 +3888,7 @@
       <c r="W40"/>
       <c r="X40"/>
     </row>
-    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>2</v>
       </c>
@@ -3359,10 +3915,10 @@
       <c r="H41" s="5">
         <v>0</v>
       </c>
-      <c r="I41" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J41" s="49"/>
+      <c r="I41" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J41" s="39"/>
       <c r="K41" s="5" t="s">
         <v>15</v>
       </c>
@@ -3374,7 +3930,7 @@
       <c r="W41"/>
       <c r="X41"/>
     </row>
-    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>3</v>
       </c>
@@ -3399,10 +3955,10 @@
       <c r="H42" s="5">
         <v>1</v>
       </c>
-      <c r="I42" s="48" t="s">
+      <c r="I42" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="J42" s="49"/>
+      <c r="J42" s="39"/>
       <c r="K42" s="5" t="s">
         <v>15</v>
       </c>
@@ -3414,7 +3970,7 @@
       <c r="W42"/>
       <c r="X42"/>
     </row>
-    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>4</v>
       </c>
@@ -3439,10 +3995,10 @@
       <c r="H43" s="5">
         <v>2</v>
       </c>
-      <c r="I43" s="48" t="s">
+      <c r="I43" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="J43" s="49"/>
+      <c r="J43" s="39"/>
       <c r="K43" s="5" t="s">
         <v>77</v>
       </c>
@@ -3454,7 +4010,7 @@
       <c r="W43"/>
       <c r="X43"/>
     </row>
-    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>5</v>
       </c>
@@ -3481,10 +4037,10 @@
       <c r="H44" s="5">
         <v>0</v>
       </c>
-      <c r="I44" s="48" t="s">
-        <v>7</v>
-      </c>
-      <c r="J44" s="49"/>
+      <c r="I44" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="J44" s="39"/>
       <c r="K44" s="5" t="s">
         <v>15</v>
       </c>
@@ -3496,7 +4052,7 @@
       <c r="W44"/>
       <c r="X44"/>
     </row>
-    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>6</v>
       </c>
@@ -3522,10 +4078,10 @@
       <c r="H45" s="5">
         <v>2</v>
       </c>
-      <c r="I45" s="48" t="s">
+      <c r="I45" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="J45" s="49"/>
+      <c r="J45" s="39"/>
       <c r="K45" s="5" t="s">
         <v>15</v>
       </c>
@@ -3537,7 +4093,7 @@
       <c r="W45"/>
       <c r="X45"/>
     </row>
-    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>7</v>
       </c>
@@ -3562,10 +4118,10 @@
       <c r="H46" s="5">
         <v>3</v>
       </c>
-      <c r="I46" s="48" t="s">
+      <c r="I46" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="J46" s="49"/>
+      <c r="J46" s="39"/>
       <c r="K46" s="5" t="s">
         <v>76</v>
       </c>
@@ -3577,7 +4133,7 @@
       <c r="W46"/>
       <c r="X46"/>
     </row>
-    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>8</v>
       </c>
@@ -3588,8 +4144,8 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="5"/>
-      <c r="I47" s="48"/>
-      <c r="J47" s="49"/>
+      <c r="I47" s="38"/>
+      <c r="J47" s="39"/>
       <c r="K47" s="5"/>
       <c r="L47" s="26"/>
       <c r="P47" s="2"/>
@@ -3597,7 +4153,7 @@
       <c r="W47"/>
       <c r="X47"/>
     </row>
-    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>9</v>
       </c>
@@ -3608,8 +4164,8 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="5"/>
-      <c r="I48" s="48"/>
-      <c r="J48" s="49"/>
+      <c r="I48" s="38"/>
+      <c r="J48" s="39"/>
       <c r="K48" s="5"/>
       <c r="L48" s="26"/>
       <c r="P48" s="2"/>
@@ -3617,7 +4173,7 @@
       <c r="W48"/>
       <c r="X48"/>
     </row>
-    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>10</v>
       </c>
@@ -3628,8 +4184,8 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="5"/>
-      <c r="I49" s="48"/>
-      <c r="J49" s="49"/>
+      <c r="I49" s="38"/>
+      <c r="J49" s="39"/>
       <c r="K49" s="5"/>
       <c r="L49" s="26"/>
       <c r="P49" s="2"/>
@@ -3637,43 +4193,32 @@
       <c r="W49"/>
       <c r="X49"/>
     </row>
-    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M50" s="2"/>
       <c r="N50" s="1"/>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M52" s="2"/>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M53" s="2"/>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M54" s="2"/>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M55" s="2"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.35">
       <c r="M56" s="2"/>
       <c r="N56" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="I39:J39"/>
-    <mergeCell ref="I40:J40"/>
-    <mergeCell ref="H32:I33"/>
-    <mergeCell ref="E34:F34"/>
     <mergeCell ref="I49:J49"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="H35:I35"/>
@@ -3686,6 +4231,17 @@
     <mergeCell ref="I47:J47"/>
     <mergeCell ref="I48:J48"/>
     <mergeCell ref="I41:J41"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="H32:I33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="G32:G33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="E32:F33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>